<commit_message>
Added test for constant vol surface.
</commit_message>
<xml_diff>
--- a/gbm/atm-volatility-surface.xlsx
+++ b/gbm/atm-volatility-surface.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitLab\stochastic_process_calibration_2022\gbm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8176BDA-9EBC-4485-BEE0-12870DF4C3D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4234764F-8378-475B-A46D-95CB91EAB8A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1FF0D0CD-0DEF-4A06-8C4A-EBD387622EDD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{1FF0D0CD-0DEF-4A06-8C4A-EBD387622EDD}"/>
   </bookViews>
   <sheets>
-    <sheet name="vol_surface" sheetId="1" r:id="rId1"/>
+    <sheet name="constant_vol_surface" sheetId="2" r:id="rId1"/>
+    <sheet name="vol_surface" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
     <t>Tenors</t>
   </si>
@@ -48,7 +49,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -193,8 +194,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,20 +509,145 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8786676B-1177-4D06-B883-E288BDA43606}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <f>1/12</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <f>2/12</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="B4" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <f>3/12</f>
+        <v>0.25</v>
+      </c>
+      <c r="B5" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <f>6/12</f>
+        <v>0.5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <f>9/12</f>
+        <v>0.75</v>
+      </c>
+      <c r="B7" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>1</v>
+      </c>
+      <c r="B8" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>2</v>
+      </c>
+      <c r="B9" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>3</v>
+      </c>
+      <c r="B10" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>5</v>
+      </c>
+      <c r="B11" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>7</v>
+      </c>
+      <c r="B12" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>10</v>
+      </c>
+      <c r="B13" s="5">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BE7F73-5F25-4DCE-B278-76EF24BAAB7F}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.36328125" customWidth="1"/>
-    <col min="2" max="2" width="9.54296875" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -529,7 +655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -537,7 +663,7 @@
         <v>12.775</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <f>1/12</f>
         <v>8.3333333333333329E-2</v>
@@ -547,7 +673,7 @@
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <f>2/12</f>
         <v>0.16666666666666666</v>
@@ -557,7 +683,7 @@
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <f>3/12</f>
         <v>0.25</v>
@@ -567,7 +693,7 @@
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <f>6/12</f>
         <v>0.5</v>
@@ -577,7 +703,7 @@
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <f>9/12</f>
         <v>0.75</v>
@@ -587,7 +713,7 @@
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>1</v>
       </c>
@@ -596,7 +722,7 @@
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>2</v>
       </c>
@@ -605,7 +731,7 @@
       </c>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>3</v>
       </c>
@@ -614,7 +740,7 @@
       </c>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>5</v>
       </c>
@@ -623,7 +749,7 @@
       </c>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>7</v>
       </c>
@@ -632,7 +758,7 @@
       </c>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>10</v>
       </c>

</xml_diff>